<commit_message>
Cleaning up. No real changes.
</commit_message>
<xml_diff>
--- a/MaleRoadStd2020.xlsx
+++ b/MaleRoadStd2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan Jones\Documents\AgeGrade\Age-Grade-Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFB40CD-DC82-4DCF-BD3C-B60C04E2D99E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9FA820-714C-4505-B54F-F416DBDFE016}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="660" windowWidth="14520" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AgeStdFactors" sheetId="1" r:id="rId1"/>
@@ -147,7 +147,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss"/>
     <numFmt numFmtId="166" formatCode="[h]:mm:ss;@"/>
-    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -504,7 +504,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -637,7 +637,7 @@
     <xf numFmtId="46" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -679,6 +679,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="46" fontId="2" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1024,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1138,7 @@
       <c r="U2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="18" t="s">
+      <c r="V2" s="60" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1191,7 +1206,7 @@
       <c r="U3" s="18">
         <v>160.93440000000001</v>
       </c>
-      <c r="V3" s="18">
+      <c r="V3" s="60">
         <v>200</v>
       </c>
     </row>
@@ -1259,7 +1274,7 @@
       <c r="U4" s="2">
         <v>39850</v>
       </c>
-      <c r="V4" s="2">
+      <c r="V4" s="55">
         <v>52800.000000000007</v>
       </c>
     </row>
@@ -1327,7 +1342,7 @@
       <c r="U5" s="4">
         <v>0.46122685185185186</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V5" s="66">
         <v>0.61111111111111116</v>
       </c>
     </row>
@@ -1395,7 +1410,7 @@
       <c r="U6" s="5">
         <v>0.60560000000000003</v>
       </c>
-      <c r="V6" s="5">
+      <c r="V6" s="67">
         <v>0.60560000000000003</v>
       </c>
     </row>
@@ -1463,7 +1478,7 @@
       <c r="U7" s="30">
         <v>0.65959999999999996</v>
       </c>
-      <c r="V7" s="30">
+      <c r="V7" s="68">
         <v>0.65959999999999996</v>
       </c>
     </row>
@@ -1531,7 +1546,7 @@
       <c r="U8" s="30">
         <v>0.70960000000000001</v>
       </c>
-      <c r="V8" s="30">
+      <c r="V8" s="68">
         <v>0.70960000000000001</v>
       </c>
     </row>
@@ -1599,7 +1614,7 @@
       <c r="U9" s="30">
         <v>0.75560000000000005</v>
       </c>
-      <c r="V9" s="30">
+      <c r="V9" s="68">
         <v>0.75560000000000005</v>
       </c>
     </row>
@@ -1667,7 +1682,7 @@
       <c r="U10" s="30">
         <v>0.79759999999999998</v>
       </c>
-      <c r="V10" s="30">
+      <c r="V10" s="68">
         <v>0.79759999999999998</v>
       </c>
     </row>
@@ -1735,7 +1750,7 @@
       <c r="U11" s="7">
         <v>0.83560000000000001</v>
       </c>
-      <c r="V11" s="7">
+      <c r="V11" s="69">
         <v>0.83560000000000001</v>
       </c>
     </row>
@@ -1803,7 +1818,7 @@
       <c r="U12" s="30">
         <v>0.86960000000000004</v>
       </c>
-      <c r="V12" s="30">
+      <c r="V12" s="68">
         <v>0.86960000000000004</v>
       </c>
     </row>
@@ -1871,7 +1886,7 @@
       <c r="U13" s="30">
         <v>0.89959999999999996</v>
       </c>
-      <c r="V13" s="30">
+      <c r="V13" s="68">
         <v>0.89959999999999996</v>
       </c>
     </row>
@@ -1939,7 +1954,7 @@
       <c r="U14" s="30">
         <v>0.92559999999999998</v>
       </c>
-      <c r="V14" s="30">
+      <c r="V14" s="68">
         <v>0.92559999999999998</v>
       </c>
     </row>
@@ -2007,7 +2022,7 @@
       <c r="U15" s="30">
         <v>0.9476</v>
       </c>
-      <c r="V15" s="30">
+      <c r="V15" s="68">
         <v>0.9476</v>
       </c>
     </row>
@@ -2075,7 +2090,7 @@
       <c r="U16" s="7">
         <v>0.96560000000000001</v>
       </c>
-      <c r="V16" s="7">
+      <c r="V16" s="69">
         <v>0.96560000000000001</v>
       </c>
     </row>
@@ -2143,7 +2158,7 @@
       <c r="U17" s="30">
         <v>0.97960000000000003</v>
       </c>
-      <c r="V17" s="30">
+      <c r="V17" s="68">
         <v>0.97960000000000003</v>
       </c>
     </row>
@@ -2211,7 +2226,7 @@
       <c r="U18" s="30">
         <v>0.99160000000000004</v>
       </c>
-      <c r="V18" s="30">
+      <c r="V18" s="68">
         <v>0.99160000000000004</v>
       </c>
     </row>
@@ -2279,7 +2294,7 @@
       <c r="U19" s="30">
         <v>0.99929999999999997</v>
       </c>
-      <c r="V19" s="30">
+      <c r="V19" s="68">
         <v>0.99929999999999997</v>
       </c>
     </row>
@@ -2347,7 +2362,7 @@
       <c r="U20" s="30">
         <v>1</v>
       </c>
-      <c r="V20" s="30">
+      <c r="V20" s="68">
         <v>1</v>
       </c>
     </row>
@@ -2415,7 +2430,7 @@
       <c r="U21" s="7">
         <v>1</v>
       </c>
-      <c r="V21" s="7">
+      <c r="V21" s="69">
         <v>1</v>
       </c>
     </row>
@@ -2483,7 +2498,7 @@
       <c r="U22" s="30">
         <v>1</v>
       </c>
-      <c r="V22" s="30">
+      <c r="V22" s="68">
         <v>1</v>
       </c>
     </row>
@@ -2551,7 +2566,7 @@
       <c r="U23" s="30">
         <v>1</v>
       </c>
-      <c r="V23" s="30">
+      <c r="V23" s="68">
         <v>1</v>
       </c>
     </row>
@@ -2619,7 +2634,7 @@
       <c r="U24" s="30">
         <v>1</v>
       </c>
-      <c r="V24" s="30">
+      <c r="V24" s="68">
         <v>1</v>
       </c>
     </row>
@@ -2687,7 +2702,7 @@
       <c r="U25" s="30">
         <v>1</v>
       </c>
-      <c r="V25" s="30">
+      <c r="V25" s="68">
         <v>1</v>
       </c>
     </row>
@@ -2755,7 +2770,7 @@
       <c r="U26" s="7">
         <v>1</v>
       </c>
-      <c r="V26" s="7">
+      <c r="V26" s="69">
         <v>1</v>
       </c>
     </row>
@@ -2823,7 +2838,7 @@
       <c r="U27" s="30">
         <v>1</v>
       </c>
-      <c r="V27" s="30">
+      <c r="V27" s="68">
         <v>1</v>
       </c>
     </row>
@@ -2891,7 +2906,7 @@
       <c r="U28" s="30">
         <v>1</v>
       </c>
-      <c r="V28" s="30">
+      <c r="V28" s="68">
         <v>1</v>
       </c>
     </row>
@@ -2959,7 +2974,7 @@
       <c r="U29" s="30">
         <v>1</v>
       </c>
-      <c r="V29" s="30">
+      <c r="V29" s="68">
         <v>1</v>
       </c>
     </row>
@@ -3027,7 +3042,7 @@
       <c r="U30" s="30">
         <v>1</v>
       </c>
-      <c r="V30" s="30">
+      <c r="V30" s="68">
         <v>1</v>
       </c>
     </row>
@@ -3095,7 +3110,7 @@
       <c r="U31" s="7">
         <v>1</v>
       </c>
-      <c r="V31" s="7">
+      <c r="V31" s="69">
         <v>1</v>
       </c>
     </row>
@@ -3163,7 +3178,7 @@
       <c r="U32" s="30">
         <v>1</v>
       </c>
-      <c r="V32" s="30">
+      <c r="V32" s="68">
         <v>1</v>
       </c>
     </row>
@@ -3231,7 +3246,7 @@
       <c r="U33" s="30">
         <v>0.99980000000000002</v>
       </c>
-      <c r="V33" s="30">
+      <c r="V33" s="68">
         <v>0.99980000000000002</v>
       </c>
     </row>
@@ -3299,7 +3314,7 @@
       <c r="U34" s="30">
         <v>0.99880000000000002</v>
       </c>
-      <c r="V34" s="30">
+      <c r="V34" s="68">
         <v>0.99880000000000002</v>
       </c>
     </row>
@@ -3367,7 +3382,7 @@
       <c r="U35" s="30">
         <v>0.99709999999999999</v>
       </c>
-      <c r="V35" s="30">
+      <c r="V35" s="68">
         <v>0.99709999999999999</v>
       </c>
     </row>
@@ -3435,7 +3450,7 @@
       <c r="U36" s="7">
         <v>0.99450000000000005</v>
       </c>
-      <c r="V36" s="7">
+      <c r="V36" s="69">
         <v>0.99450000000000005</v>
       </c>
     </row>
@@ -3503,7 +3518,7 @@
       <c r="U37" s="30">
         <v>0.99109999999999998</v>
       </c>
-      <c r="V37" s="30">
+      <c r="V37" s="68">
         <v>0.99109999999999998</v>
       </c>
     </row>
@@ -3571,7 +3586,7 @@
       <c r="U38" s="30">
         <v>0.98699999999999999</v>
       </c>
-      <c r="V38" s="30">
+      <c r="V38" s="68">
         <v>0.98699999999999999</v>
       </c>
     </row>
@@ -3639,7 +3654,7 @@
       <c r="U39" s="30">
         <v>0.98199999999999998</v>
       </c>
-      <c r="V39" s="30">
+      <c r="V39" s="68">
         <v>0.98199999999999998</v>
       </c>
     </row>
@@ -3707,7 +3722,7 @@
       <c r="U40" s="30">
         <v>0.97619999999999996</v>
       </c>
-      <c r="V40" s="30">
+      <c r="V40" s="68">
         <v>0.97619999999999996</v>
       </c>
     </row>
@@ -3775,7 +3790,7 @@
       <c r="U41" s="7">
         <v>0.96960000000000002</v>
       </c>
-      <c r="V41" s="7">
+      <c r="V41" s="69">
         <v>0.96960000000000002</v>
       </c>
     </row>
@@ -3843,7 +3858,7 @@
       <c r="U42" s="30">
         <v>0.96230000000000004</v>
       </c>
-      <c r="V42" s="30">
+      <c r="V42" s="68">
         <v>0.96230000000000004</v>
       </c>
     </row>
@@ -3911,7 +3926,7 @@
       <c r="U43" s="30">
         <v>0.95450000000000002</v>
       </c>
-      <c r="V43" s="30">
+      <c r="V43" s="68">
         <v>0.95450000000000002</v>
       </c>
     </row>
@@ -3979,7 +3994,7 @@
       <c r="U44" s="30">
         <v>0.94669999999999999</v>
       </c>
-      <c r="V44" s="30">
+      <c r="V44" s="68">
         <v>0.94669999999999999</v>
       </c>
     </row>
@@ -4047,7 +4062,7 @@
       <c r="U45" s="30">
         <v>0.93889999999999996</v>
       </c>
-      <c r="V45" s="30">
+      <c r="V45" s="68">
         <v>0.93889999999999996</v>
       </c>
     </row>
@@ -4115,7 +4130,7 @@
       <c r="U46" s="7">
         <v>0.93110000000000004</v>
       </c>
-      <c r="V46" s="7">
+      <c r="V46" s="69">
         <v>0.93110000000000004</v>
       </c>
     </row>
@@ -4183,7 +4198,7 @@
       <c r="U47" s="30">
         <v>0.9234</v>
       </c>
-      <c r="V47" s="30">
+      <c r="V47" s="68">
         <v>0.9234</v>
       </c>
     </row>
@@ -4251,7 +4266,7 @@
       <c r="U48" s="30">
         <v>0.91559999999999997</v>
       </c>
-      <c r="V48" s="30">
+      <c r="V48" s="68">
         <v>0.91559999999999997</v>
       </c>
     </row>
@@ -4319,7 +4334,7 @@
       <c r="U49" s="30">
         <v>0.90780000000000005</v>
       </c>
-      <c r="V49" s="30">
+      <c r="V49" s="68">
         <v>0.90780000000000005</v>
       </c>
     </row>
@@ -4387,7 +4402,7 @@
       <c r="U50" s="30">
         <v>0.9</v>
       </c>
-      <c r="V50" s="30">
+      <c r="V50" s="68">
         <v>0.9</v>
       </c>
     </row>
@@ -4455,7 +4470,7 @@
       <c r="U51" s="7">
         <v>0.89219999999999999</v>
       </c>
-      <c r="V51" s="7">
+      <c r="V51" s="69">
         <v>0.89219999999999999</v>
       </c>
     </row>
@@ -4523,7 +4538,7 @@
       <c r="U52" s="30">
         <v>0.88449999999999995</v>
       </c>
-      <c r="V52" s="30">
+      <c r="V52" s="68">
         <v>0.88449999999999995</v>
       </c>
     </row>
@@ -4591,7 +4606,7 @@
       <c r="U53" s="30">
         <v>0.87670000000000003</v>
       </c>
-      <c r="V53" s="30">
+      <c r="V53" s="68">
         <v>0.87670000000000003</v>
       </c>
     </row>
@@ -4659,7 +4674,7 @@
       <c r="U54" s="30">
         <v>0.86890000000000001</v>
       </c>
-      <c r="V54" s="30">
+      <c r="V54" s="68">
         <v>0.86890000000000001</v>
       </c>
     </row>
@@ -4727,7 +4742,7 @@
       <c r="U55" s="30">
         <v>0.86109999999999998</v>
       </c>
-      <c r="V55" s="30">
+      <c r="V55" s="68">
         <v>0.86109999999999998</v>
       </c>
     </row>
@@ -4795,7 +4810,7 @@
       <c r="U56" s="7">
         <v>0.85329999999999995</v>
       </c>
-      <c r="V56" s="7">
+      <c r="V56" s="69">
         <v>0.85329999999999995</v>
       </c>
     </row>
@@ -4863,7 +4878,7 @@
       <c r="U57" s="30">
         <v>0.84560000000000002</v>
       </c>
-      <c r="V57" s="30">
+      <c r="V57" s="68">
         <v>0.84560000000000002</v>
       </c>
     </row>
@@ -4931,7 +4946,7 @@
       <c r="U58" s="30">
         <v>0.83779999999999999</v>
       </c>
-      <c r="V58" s="30">
+      <c r="V58" s="68">
         <v>0.83779999999999999</v>
       </c>
     </row>
@@ -4999,7 +5014,7 @@
       <c r="U59" s="30">
         <v>0.83</v>
       </c>
-      <c r="V59" s="30">
+      <c r="V59" s="68">
         <v>0.83</v>
       </c>
     </row>
@@ -5067,7 +5082,7 @@
       <c r="U60" s="30">
         <v>0.82220000000000004</v>
       </c>
-      <c r="V60" s="30">
+      <c r="V60" s="68">
         <v>0.82220000000000004</v>
       </c>
     </row>
@@ -5135,7 +5150,7 @@
       <c r="U61" s="7">
         <v>0.81440000000000001</v>
       </c>
-      <c r="V61" s="7">
+      <c r="V61" s="69">
         <v>0.81440000000000001</v>
       </c>
     </row>
@@ -5203,7 +5218,7 @@
       <c r="U62" s="30">
         <v>0.80669999999999997</v>
       </c>
-      <c r="V62" s="30">
+      <c r="V62" s="68">
         <v>0.80669999999999997</v>
       </c>
     </row>
@@ -5271,7 +5286,7 @@
       <c r="U63" s="30">
         <v>0.79890000000000005</v>
       </c>
-      <c r="V63" s="30">
+      <c r="V63" s="68">
         <v>0.79890000000000005</v>
       </c>
     </row>
@@ -5339,7 +5354,7 @@
       <c r="U64" s="30">
         <v>0.79110000000000003</v>
       </c>
-      <c r="V64" s="30">
+      <c r="V64" s="68">
         <v>0.79110000000000003</v>
       </c>
     </row>
@@ -5407,7 +5422,7 @@
       <c r="U65" s="30">
         <v>0.7833</v>
       </c>
-      <c r="V65" s="30">
+      <c r="V65" s="68">
         <v>0.7833</v>
       </c>
     </row>
@@ -5475,7 +5490,7 @@
       <c r="U66" s="7">
         <v>0.77549999999999997</v>
       </c>
-      <c r="V66" s="7">
+      <c r="V66" s="69">
         <v>0.77549999999999997</v>
       </c>
     </row>
@@ -5543,7 +5558,7 @@
       <c r="U67" s="30">
         <v>0.76780000000000004</v>
       </c>
-      <c r="V67" s="30">
+      <c r="V67" s="68">
         <v>0.76780000000000004</v>
       </c>
     </row>
@@ -5611,7 +5626,7 @@
       <c r="U68" s="30">
         <v>0.76</v>
       </c>
-      <c r="V68" s="30">
+      <c r="V68" s="68">
         <v>0.76</v>
       </c>
     </row>
@@ -5679,7 +5694,7 @@
       <c r="U69" s="30">
         <v>0.75219999999999998</v>
       </c>
-      <c r="V69" s="30">
+      <c r="V69" s="68">
         <v>0.75219999999999998</v>
       </c>
     </row>
@@ -5747,7 +5762,7 @@
       <c r="U70" s="30">
         <v>0.74439999999999995</v>
       </c>
-      <c r="V70" s="30">
+      <c r="V70" s="68">
         <v>0.74439999999999995</v>
       </c>
     </row>
@@ -5815,7 +5830,7 @@
       <c r="U71" s="7">
         <v>0.73660000000000003</v>
       </c>
-      <c r="V71" s="7">
+      <c r="V71" s="69">
         <v>0.73660000000000003</v>
       </c>
     </row>
@@ -5883,7 +5898,7 @@
       <c r="U72" s="30">
         <v>0.72860000000000003</v>
       </c>
-      <c r="V72" s="30">
+      <c r="V72" s="68">
         <v>0.72860000000000003</v>
       </c>
     </row>
@@ -5951,7 +5966,7 @@
       <c r="U73" s="30">
         <v>0.7198</v>
       </c>
-      <c r="V73" s="30">
+      <c r="V73" s="68">
         <v>0.7198</v>
       </c>
     </row>
@@ -6019,7 +6034,7 @@
       <c r="U74" s="30">
         <v>0.71040000000000003</v>
       </c>
-      <c r="V74" s="30">
+      <c r="V74" s="68">
         <v>0.71040000000000003</v>
       </c>
     </row>
@@ -6087,7 +6102,7 @@
       <c r="U75" s="30">
         <v>0.70020000000000004</v>
       </c>
-      <c r="V75" s="30">
+      <c r="V75" s="68">
         <v>0.70020000000000004</v>
       </c>
     </row>
@@ -6155,7 +6170,7 @@
       <c r="U76" s="7">
         <v>0.68930000000000002</v>
       </c>
-      <c r="V76" s="7">
+      <c r="V76" s="69">
         <v>0.68930000000000002</v>
       </c>
     </row>
@@ -6223,7 +6238,7 @@
       <c r="U77" s="30">
         <v>0.67779999999999996</v>
       </c>
-      <c r="V77" s="30">
+      <c r="V77" s="68">
         <v>0.67779999999999996</v>
       </c>
     </row>
@@ -6291,7 +6306,7 @@
       <c r="U78" s="30">
         <v>0.66549999999999998</v>
       </c>
-      <c r="V78" s="30">
+      <c r="V78" s="68">
         <v>0.66549999999999998</v>
       </c>
     </row>
@@ -6359,7 +6374,7 @@
       <c r="U79" s="30">
         <v>0.65259999999999996</v>
       </c>
-      <c r="V79" s="30">
+      <c r="V79" s="68">
         <v>0.65259999999999996</v>
       </c>
     </row>
@@ -6427,7 +6442,7 @@
       <c r="U80" s="30">
         <v>0.63890000000000002</v>
       </c>
-      <c r="V80" s="30">
+      <c r="V80" s="68">
         <v>0.63890000000000002</v>
       </c>
     </row>
@@ -6495,7 +6510,7 @@
       <c r="U81" s="7">
         <v>0.62450000000000006</v>
       </c>
-      <c r="V81" s="7">
+      <c r="V81" s="69">
         <v>0.62450000000000006</v>
       </c>
     </row>
@@ -6563,7 +6578,7 @@
       <c r="U82" s="30">
         <v>0.60950000000000004</v>
       </c>
-      <c r="V82" s="30">
+      <c r="V82" s="68">
         <v>0.60950000000000004</v>
       </c>
     </row>
@@ -6631,7 +6646,7 @@
       <c r="U83" s="30">
         <v>0.59370000000000001</v>
       </c>
-      <c r="V83" s="30">
+      <c r="V83" s="68">
         <v>0.59370000000000001</v>
       </c>
     </row>
@@ -6699,7 +6714,7 @@
       <c r="U84" s="30">
         <v>0.57730000000000004</v>
       </c>
-      <c r="V84" s="30">
+      <c r="V84" s="68">
         <v>0.57730000000000004</v>
       </c>
     </row>
@@ -6767,7 +6782,7 @@
       <c r="U85" s="30">
         <v>0.56010000000000004</v>
       </c>
-      <c r="V85" s="30">
+      <c r="V85" s="68">
         <v>0.56010000000000004</v>
       </c>
     </row>
@@ -6835,7 +6850,7 @@
       <c r="U86" s="7">
         <v>0.54220000000000002</v>
       </c>
-      <c r="V86" s="7">
+      <c r="V86" s="69">
         <v>0.54220000000000002</v>
       </c>
     </row>
@@ -6903,7 +6918,7 @@
       <c r="U87" s="30">
         <v>0.52370000000000005</v>
       </c>
-      <c r="V87" s="30">
+      <c r="V87" s="68">
         <v>0.52370000000000005</v>
       </c>
     </row>
@@ -6971,7 +6986,7 @@
       <c r="U88" s="30">
         <v>0.50439999999999996</v>
       </c>
-      <c r="V88" s="30">
+      <c r="V88" s="68">
         <v>0.50439999999999996</v>
       </c>
     </row>
@@ -7039,7 +7054,7 @@
       <c r="U89" s="30">
         <v>0.48449999999999999</v>
       </c>
-      <c r="V89" s="30">
+      <c r="V89" s="68">
         <v>0.48449999999999999</v>
       </c>
     </row>
@@ -7107,7 +7122,7 @@
       <c r="U90" s="30">
         <v>0.46379999999999999</v>
       </c>
-      <c r="V90" s="30">
+      <c r="V90" s="68">
         <v>0.46379999999999999</v>
       </c>
     </row>
@@ -7175,7 +7190,7 @@
       <c r="U91" s="7">
         <v>0.44240000000000002</v>
       </c>
-      <c r="V91" s="7">
+      <c r="V91" s="69">
         <v>0.44240000000000002</v>
       </c>
     </row>
@@ -7243,7 +7258,7 @@
       <c r="U92" s="30">
         <v>0.4204</v>
       </c>
-      <c r="V92" s="30">
+      <c r="V92" s="68">
         <v>0.4204</v>
       </c>
     </row>
@@ -7311,7 +7326,7 @@
       <c r="U93" s="30">
         <v>0.39760000000000001</v>
       </c>
-      <c r="V93" s="30">
+      <c r="V93" s="68">
         <v>0.39760000000000001</v>
       </c>
     </row>
@@ -7379,7 +7394,7 @@
       <c r="U94" s="30">
         <v>0.37419999999999998</v>
       </c>
-      <c r="V94" s="30">
+      <c r="V94" s="68">
         <v>0.37419999999999998</v>
       </c>
     </row>
@@ -7447,7 +7462,7 @@
       <c r="U95" s="30">
         <v>0.35</v>
       </c>
-      <c r="V95" s="30">
+      <c r="V95" s="68">
         <v>0.35</v>
       </c>
     </row>
@@ -7515,7 +7530,7 @@
       <c r="U96" s="7">
         <v>0.3251</v>
       </c>
-      <c r="V96" s="7">
+      <c r="V96" s="69">
         <v>0.3251</v>
       </c>
     </row>
@@ -7583,7 +7598,7 @@
       <c r="U97" s="30">
         <v>0.29959999999999998</v>
       </c>
-      <c r="V97" s="30">
+      <c r="V97" s="68">
         <v>0.29959999999999998</v>
       </c>
     </row>
@@ -7651,7 +7666,7 @@
       <c r="U98" s="30">
         <v>0.27329999999999999</v>
       </c>
-      <c r="V98" s="30">
+      <c r="V98" s="68">
         <v>0.27329999999999999</v>
       </c>
     </row>
@@ -7719,7 +7734,7 @@
       <c r="U99" s="30">
         <v>0.24640000000000001</v>
       </c>
-      <c r="V99" s="30">
+      <c r="V99" s="68">
         <v>0.24640000000000001</v>
       </c>
     </row>
@@ -7787,7 +7802,7 @@
       <c r="U100" s="30">
         <v>0.21870000000000001</v>
       </c>
-      <c r="V100" s="30">
+      <c r="V100" s="68">
         <v>0.21870000000000001</v>
       </c>
     </row>
@@ -7855,7 +7870,7 @@
       <c r="U101" s="7">
         <v>0.1903</v>
       </c>
-      <c r="V101" s="7">
+      <c r="V101" s="70">
         <v>0.1903</v>
       </c>
     </row>

</xml_diff>